<commit_message>
Started Adaptation to CS-Cart 4.18.2a. Updated pom.xml. Changed using of HSSF on XHHF and it helps me to use simple .xlsx file on my test.
</commit_message>
<xml_diff>
--- a/01 Settings - TestCase01_CategoryPage_GridTest.xlsx
+++ b/01 Settings - TestCase01_CategoryPage_GridTest.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IDEA Projects\UniTheme2_Pairwise\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A6A13C-7709-4C57-9FA8-3386C8537970}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Настройки и Условия" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Коды значений" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Настройки и Условия" sheetId="1" r:id="rId1"/>
+    <sheet name="Коды значений" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,12 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
-  <si>
-    <t xml:space="preserve">Страница категории “Сетка”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Настройки цветосхемы</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
+  <si>
+    <t>Страница категории “Сетка”</t>
+  </si>
+  <si>
+    <t>Настройки цветосхемы</t>
   </si>
   <si>
     <t xml:space="preserve">Round corners for interface elements </t>
@@ -44,10 +49,10 @@
     <t xml:space="preserve">Display headers in capital letters </t>
   </si>
   <si>
-    <t xml:space="preserve">on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">off</t>
+    <t>on</t>
+  </si>
+  <si>
+    <t>off</t>
   </si>
   <si>
     <t xml:space="preserve">Display text in capital letters </t>
@@ -71,10 +76,10 @@
     <t xml:space="preserve">Use elements alignment </t>
   </si>
   <si>
-    <t xml:space="preserve">use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">don’t use</t>
+    <t>use</t>
+  </si>
+  <si>
+    <t>don’t use</t>
   </si>
   <si>
     <t xml:space="preserve">Expand grid item on hover </t>
@@ -83,13 +88,13 @@
     <t xml:space="preserve">Font weight for product name </t>
   </si>
   <si>
-    <t xml:space="preserve">Normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Настройки темы</t>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Bold</t>
+  </si>
+  <si>
+    <t>Настройки темы</t>
   </si>
   <si>
     <t xml:space="preserve">Decolorize out of stock products </t>
@@ -182,239 +187,245 @@
     <t xml:space="preserve">Do not switch </t>
   </si>
   <si>
-    <t xml:space="preserve">With dots</t>
+    <t>With dots</t>
   </si>
   <si>
     <t xml:space="preserve">With stripes </t>
   </si>
   <si>
-    <t xml:space="preserve">Условия подготовки:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар без наличия</t>
-  </si>
-  <si>
-    <t xml:space="preserve">все эти товары можно взять из категории HTC и работать только с этой категорией</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар без наличия и с действием “Предзаказ”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар без цены</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар без цены и с действием “Попросить покупателя ввести цену”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар со скидкой</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Подготовить бренд — вывод логотипа на стр категории</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Коды цветосхемы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_RCFIE_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_RCFIE_Little</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_RCFIE_Fully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_DHICL_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_DHICL_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_DTICL_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_DTICL_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_FTPG_Not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_FTPG_Without</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_FTPG_With</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_ABMFPI_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_ABMFPI_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_UEA_Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_UEA_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_EGIOH_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_EGIOH_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_FWFPN_Normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ColSch_FWFPN_Bold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Коды настроек темы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DOOSP_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DOOSP_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_PDF_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_PDF_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_PDF_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_PDF_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPATT_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPATT_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DESOPR_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DESOPR_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DCVOPR_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DCVOPR_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_NOLITPN_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_NOLITPN_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_NOLITPN_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_NOLITPN_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPC_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPC_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DAS_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DAS_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SQC_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SQC_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SATCB_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SATCB_Simplified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SATCB_Icon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SATCB_Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SATCB_Both</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_Desc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_Variations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_DescAndVar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_API_FeatAndVar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SAIOH_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SAIOH_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SBL_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SBL_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SYS_On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SYS_Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SSIG_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SSIG_Dots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SSIG_Arrows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPIWHMP_Dont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPIWHMP_Dots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_SPIWHMP_Stripes</t>
+    <t>Условия подготовки:</t>
+  </si>
+  <si>
+    <t>Товар без наличия</t>
+  </si>
+  <si>
+    <t>все эти товары можно взять из категории HTC и работать только с этой категорией</t>
+  </si>
+  <si>
+    <t>Товар без наличия и с действием “Предзаказ”</t>
+  </si>
+  <si>
+    <t>Товар без цены</t>
+  </si>
+  <si>
+    <t>Товар без цены и с действием “Попросить покупателя ввести цену”</t>
+  </si>
+  <si>
+    <t>Товар со скидкой</t>
+  </si>
+  <si>
+    <t>Подготовить бренд — вывод логотипа на стр категории</t>
+  </si>
+  <si>
+    <t>Коды цветосхемы</t>
+  </si>
+  <si>
+    <t>ColSch_RCFIE_Dont</t>
+  </si>
+  <si>
+    <t>ColSch_RCFIE_Little</t>
+  </si>
+  <si>
+    <t>ColSch_RCFIE_Fully</t>
+  </si>
+  <si>
+    <t>ColSch_DHICL_On</t>
+  </si>
+  <si>
+    <t>ColSch_DHICL_Off</t>
+  </si>
+  <si>
+    <t>ColSch_DTICL_On</t>
+  </si>
+  <si>
+    <t>ColSch_DTICL_Off</t>
+  </si>
+  <si>
+    <t>ColSch_FTPG_Not</t>
+  </si>
+  <si>
+    <t>ColSch_FTPG_Without</t>
+  </si>
+  <si>
+    <t>ColSch_FTPG_With</t>
+  </si>
+  <si>
+    <t>ColSch_ABMFPI_On</t>
+  </si>
+  <si>
+    <t>ColSch_ABMFPI_Off</t>
+  </si>
+  <si>
+    <t>ColSch_UEA_Use</t>
+  </si>
+  <si>
+    <t>ColSch_UEA_Dont</t>
+  </si>
+  <si>
+    <t>ColSch_EGIOH_On</t>
+  </si>
+  <si>
+    <t>ColSch_EGIOH_Off</t>
+  </si>
+  <si>
+    <t>ColSch_FWFPN_Normal</t>
+  </si>
+  <si>
+    <t>ColSch_FWFPN_Bold</t>
+  </si>
+  <si>
+    <t>Коды настроек темы</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DOOSP_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DOOSP_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_PDF_1</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_PDF_2</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_PDF_3</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_PDF_4</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPATT_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPATT_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DESOPR_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DESOPR_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DCVOPR_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DCVOPR_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_NOLITPN_1</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_NOLITPN_2</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_NOLITPN_3</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_NOLITPN_4</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPC_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPC_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DAS_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_DAS_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SQC_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SQC_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SATCB_Dont</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SATCB_Simplified</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SATCB_Icon</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SATCB_Text</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SATCB_Both</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_Dont</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_Desc</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_Features</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_Variations</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_DescAndVar</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_API_FeatAndVar</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SAIOH_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SAIOH_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SBL_On</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SBL_Off</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SSIG_Dont</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SSIG_Dots</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SSIG_Arrows</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPIWHMP_Dont</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPIWHMP_Dots</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SPIWHMP_Stripes</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SYS_Dont</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SYS_Full</t>
+  </si>
+  <si>
+    <t>ThemeProductLists_SYS_Short</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -422,32 +433,14 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -460,16 +453,22 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -477,115 +476,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -638,42 +612,41 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.81"/>
+    <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -687,7 +660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -698,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -709,7 +682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -723,7 +696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -734,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -745,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -756,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -767,12 +740,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -783,24 +756,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="1">
         <v>3</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
@@ -811,7 +784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -822,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -833,24 +806,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
@@ -861,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
@@ -872,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -883,7 +856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
@@ -903,7 +876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -926,7 +899,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
@@ -937,7 +910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
@@ -948,18 +921,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
@@ -973,7 +949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
@@ -987,12 +963,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
@@ -1000,39 +976,38 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
   </headerFooter>
@@ -1040,33 +1015,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.39"/>
+    <col min="1" max="1" width="42.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1080,7 +1052,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1063,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1074,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1088,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1127,7 +1099,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1110,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1121,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1160,12 +1132,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1176,7 +1148,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -1193,7 +1165,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1176,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1215,7 +1187,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1226,7 +1198,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1243,7 +1215,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1254,7 +1226,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -1265,7 +1237,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1276,7 +1248,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
@@ -1296,7 +1268,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1319,7 +1291,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
@@ -1330,7 +1302,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
@@ -1341,50 +1313,52 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>127</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CСтраница &amp;P</oddFooter>
   </headerFooter>

</xml_diff>